<commit_message>
Add modified hours into pages
</commit_message>
<xml_diff>
--- a/backend/routes/exportAttendeeData/csvAttendeesRequested/event-65fdd2c0ce313a0eb206bc6c-attendees.xlsx
+++ b/backend/routes/exportAttendeeData/csvAttendeesRequested/event-65fdd2c0ce313a0eb206bc6c-attendees.xlsx
@@ -40,10 +40,10 @@
     <x:t>65616a1011a2035f14571238</x:t>
   </x:si>
   <x:si>
-    <x:t>Robby</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jonas</x:t>
+    <x:t>Joe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jonas2</x:t>
   </x:si>
   <x:si>
     <x:t>noahseligson18@gmail.com</x:t>
@@ -55,7 +55,7 @@
     <x:t>Tue Jan 09 2024 16:01:17 GMT-0500 (Eastern Standard Time)</x:t>
   </x:si>
   <x:si>
-    <x:t>Dance &amp; Movement, Education, Technology, Environment, Sports &amp; Recreation, Coding &amp; Software Development, Music &amp; Performance, Animal Welfare, Health &amp; Wellness</x:t>
+    <x:t>Education, Technology, Environment, Sports &amp; Recreation, Coding &amp; Software Development, Music &amp; Performance, Health &amp; Wellness, Animal Welfare</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>